<commit_message>
Update Bill of Materials ECE 411.xlsx
added received/received qty/value columns to BOM. Updated to parts we have at Josh's house.
</commit_message>
<xml_diff>
--- a/Bill of Materials ECE 411.xlsx
+++ b/Bill of Materials ECE 411.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdworning\Documents\GitHub\Window-weather-Monitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8DF0C7-E469-4A8A-8AA4-CF8C58EBD6BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9245DE4B-E04E-492A-A68B-4D36BBFD6FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="184">
   <si>
     <t>Bill Of Materials for: [TEAM 4] [Window Weather Monitor]</t>
   </si>
@@ -513,6 +513,78 @@
   </si>
   <si>
     <t>KOA Speer Electronics</t>
+  </si>
+  <si>
+    <t>2.0r1</t>
+  </si>
+  <si>
+    <t>Updated BOM to add part values where applicable. Also added received section.</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>0.1uF</t>
+  </si>
+  <si>
+    <t>22uF</t>
+  </si>
+  <si>
+    <t>0.022uF</t>
+  </si>
+  <si>
+    <t>3V</t>
+  </si>
+  <si>
+    <t>100UF</t>
+  </si>
+  <si>
+    <t>10UF</t>
+  </si>
+  <si>
+    <t>RED</t>
+  </si>
+  <si>
+    <t>GREEN</t>
+  </si>
+  <si>
+    <t>RGBK</t>
+  </si>
+  <si>
+    <t>0 Ohm</t>
+  </si>
+  <si>
+    <t>5K Ohm</t>
+  </si>
+  <si>
+    <t>4.7 kOhm</t>
+  </si>
+  <si>
+    <t>121 Ohm</t>
+  </si>
+  <si>
+    <t>430 Ohm</t>
+  </si>
+  <si>
+    <t>100 Ohm</t>
+  </si>
+  <si>
+    <t>33 kOhm</t>
+  </si>
+  <si>
+    <t>5 kOHM</t>
+  </si>
+  <si>
+    <t>Received (Y/N)</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Received QTY</t>
   </si>
 </sst>
 </file>
@@ -576,7 +648,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -584,12 +656,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -607,38 +694,287 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="22">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -849,28 +1185,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC986"/>
+  <dimension ref="A1:AD986"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="5.140625" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="26.42578125" customWidth="1"/>
-    <col min="7" max="7" width="49.28515625" customWidth="1"/>
-    <col min="8" max="8" width="9" customWidth="1"/>
-    <col min="9" max="9" width="20.85546875" customWidth="1"/>
-    <col min="10" max="11" width="8.7109375" customWidth="1"/>
-    <col min="23" max="23" width="14.42578125" style="13"/>
+    <col min="3" max="3" width="48.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="26.42578125" customWidth="1"/>
+    <col min="8" max="8" width="49.28515625" customWidth="1"/>
+    <col min="9" max="9" width="9" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" customWidth="1"/>
+    <col min="11" max="12" width="8.7109375" customWidth="1"/>
+    <col min="13" max="13" width="8.28515625" style="17" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -882,10 +1220,12 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-      <c r="J1" s="2"/>
+      <c r="J1" s="1"/>
       <c r="K1" s="2"/>
-    </row>
-    <row r="2" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L1" s="2"/>
+      <c r="N1"/>
+    </row>
+    <row r="2" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -896,39 +1236,45 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
-      <c r="J2" s="4"/>
+      <c r="I2" s="3"/>
       <c r="K2" s="4"/>
-    </row>
-    <row r="3" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L2" s="4"/>
+      <c r="N2"/>
+    </row>
+    <row r="3" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="E3" s="3"/>
       <c r="H3" s="3"/>
-      <c r="J3" s="4"/>
+      <c r="I3" s="3"/>
       <c r="K3" s="4"/>
-    </row>
-    <row r="4" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L3" s="4"/>
+      <c r="N3"/>
+    </row>
+    <row r="4" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="3"/>
       <c r="H4" s="3"/>
-      <c r="J4" s="4"/>
+      <c r="I4" s="3"/>
       <c r="K4" s="4"/>
-    </row>
-    <row r="5" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L4" s="4"/>
+      <c r="N4"/>
+    </row>
+    <row r="5" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -937,1313 +1283,1512 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="J5" s="4"/>
+      <c r="I5" s="3"/>
       <c r="K5" s="4"/>
-    </row>
-    <row r="6" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="L5" s="4"/>
+      <c r="N5"/>
+    </row>
+    <row r="6" spans="1:23" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="E6" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="H6" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="I6" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="J6" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="K6" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="L6" s="34" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="20">
+      <c r="M6" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="N6" s="34" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="21">
         <v>1</v>
       </c>
-      <c r="B7" s="20">
+      <c r="B7" s="21">
         <v>1</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="23"/>
+      <c r="E7" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="G7" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="21" t="s">
+      <c r="J7" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="J7" s="4">
+      <c r="K7" s="27">
         <v>2.06</v>
       </c>
-      <c r="K7" s="4">
-        <f t="shared" ref="K7:K12" si="0">J7*A7</f>
+      <c r="L7" s="27">
+        <f t="shared" ref="L7:M12" si="0">K7*A7</f>
         <v>2.06</v>
       </c>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="3"/>
+      <c r="M7" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="N7" s="36">
+        <v>3</v>
+      </c>
+      <c r="O7" s="17"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="8"/>
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
-      <c r="V7" s="4"/>
-    </row>
-    <row r="8" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="20">
+      <c r="V7" s="3"/>
+      <c r="W7" s="4"/>
+    </row>
+    <row r="8" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="21">
         <v>2</v>
       </c>
-      <c r="B8" s="20">
+      <c r="B8" s="21">
         <v>3</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="E8" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="22" t="s">
+      <c r="J8" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="J8">
+      <c r="K8" s="23">
         <v>0.1</v>
       </c>
-      <c r="K8" s="4">
+      <c r="L8" s="27">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
-      <c r="U8" s="15"/>
-    </row>
-    <row r="9" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="20">
+      <c r="M8" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="N8" s="36"/>
+      <c r="O8" s="17"/>
+      <c r="V8" s="14"/>
+    </row>
+    <row r="9" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="21">
         <v>3</v>
       </c>
-      <c r="B9" s="20">
+      <c r="B9" s="21">
         <v>3</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="E9" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="F9" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="H9" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="I9" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="22" t="s">
+      <c r="J9" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="J9">
+      <c r="K9" s="23">
         <v>0.74</v>
       </c>
-      <c r="K9" s="4">
+      <c r="L9" s="27">
         <f t="shared" si="0"/>
         <v>2.2199999999999998</v>
       </c>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
-      <c r="S9" s="14"/>
-      <c r="T9" s="14"/>
-      <c r="U9" s="15"/>
-    </row>
-    <row r="10" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="20">
+      <c r="M9" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="N9" s="36"/>
+      <c r="O9" s="17"/>
+      <c r="T9" s="13"/>
+      <c r="U9" s="13"/>
+      <c r="V9" s="14"/>
+    </row>
+    <row r="10" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="21">
         <v>4</v>
       </c>
-      <c r="B10" s="20">
+      <c r="B10" s="21">
         <v>1</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="E10" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="F10" s="30" t="s">
         <v>155</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="G10" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="H10" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="I10" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="22" t="s">
+      <c r="J10" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="J10">
+      <c r="K10" s="23">
         <v>0.1</v>
       </c>
-      <c r="K10" s="4">
+      <c r="L10" s="27">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
-      <c r="R10" s="16"/>
-      <c r="S10" s="14"/>
-      <c r="T10" s="14"/>
-      <c r="U10" s="15"/>
-    </row>
-    <row r="11" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="20">
+      <c r="M10" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="N10" s="36"/>
+      <c r="O10" s="17"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="13"/>
+      <c r="U10" s="13"/>
+      <c r="V10" s="14"/>
+    </row>
+    <row r="11" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="21">
         <v>5</v>
       </c>
-      <c r="B11" s="20">
+      <c r="B11" s="21">
         <v>1</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="E11" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="F11" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="H11" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="H11" s="14" t="s">
+      <c r="I11" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="22" t="s">
+      <c r="J11" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="J11">
+      <c r="K11" s="23">
         <v>0.42</v>
       </c>
-      <c r="K11" s="4">
+      <c r="L11" s="27">
         <f t="shared" si="0"/>
         <v>2.1</v>
       </c>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
-      <c r="S11" s="14"/>
-      <c r="T11" s="14"/>
-      <c r="U11" s="15"/>
-    </row>
-    <row r="12" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="20">
+      <c r="M11" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="N11" s="36">
+        <v>0</v>
+      </c>
+      <c r="O11" s="17"/>
+      <c r="T11" s="13"/>
+      <c r="U11" s="13"/>
+      <c r="V11" s="14"/>
+    </row>
+    <row r="12" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="21">
         <v>6</v>
       </c>
-      <c r="B12" s="20">
+      <c r="B12" s="21">
         <v>1</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="E12" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="F12" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="H12" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="I12" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="I12" s="22" t="s">
+      <c r="J12" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="J12">
+      <c r="K12" s="23">
         <v>0.32</v>
       </c>
-      <c r="K12" s="4">
+      <c r="L12" s="27">
         <f t="shared" si="0"/>
         <v>1.92</v>
       </c>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19"/>
-      <c r="S12" s="14"/>
-      <c r="T12" s="14"/>
-      <c r="U12" s="15"/>
-    </row>
-    <row r="13" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="20">
+      <c r="M12" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="N12" s="36"/>
+      <c r="O12" s="17"/>
+      <c r="T12" s="13"/>
+      <c r="U12" s="13"/>
+      <c r="V12" s="14"/>
+    </row>
+    <row r="13" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="21">
         <v>7</v>
       </c>
-      <c r="B13" s="20">
+      <c r="B13" s="21">
         <v>1</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="E13" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="F13" s="30" t="s">
         <v>156</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="H13" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="I13" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="I13" s="22" t="s">
+      <c r="J13" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="J13">
+      <c r="K13" s="23">
         <v>0.32</v>
       </c>
-      <c r="K13" s="4">
-        <f>J13*B13</f>
+      <c r="L13" s="27">
+        <f>K13*B13</f>
         <v>0.32</v>
       </c>
-      <c r="M13" s="19"/>
-      <c r="N13" s="19"/>
-      <c r="S13" s="14"/>
-      <c r="T13" s="14"/>
-      <c r="U13" s="15"/>
-    </row>
-    <row r="14" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="20">
+      <c r="M13" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="N13" s="36">
+        <v>3</v>
+      </c>
+      <c r="O13" s="17"/>
+      <c r="T13" s="13"/>
+      <c r="U13" s="13"/>
+      <c r="V13" s="14"/>
+    </row>
+    <row r="14" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="21">
         <v>8</v>
       </c>
-      <c r="B14" s="20">
+      <c r="B14" s="21">
         <v>1</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="E14" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="F14" s="30" t="s">
         <v>156</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="H14" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="I14" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="I14" s="22" t="s">
+      <c r="J14" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="J14">
+      <c r="K14" s="23">
         <v>0.31</v>
       </c>
-      <c r="K14" s="4">
-        <f t="shared" ref="K14:K36" si="1">J14*B14</f>
+      <c r="L14" s="27">
+        <f t="shared" ref="L14:M36" si="1">K14*B14</f>
         <v>0.31</v>
       </c>
-      <c r="M14" s="19"/>
-      <c r="N14" s="19"/>
-      <c r="S14" s="14"/>
-      <c r="T14" s="14"/>
-      <c r="U14" s="15"/>
-    </row>
-    <row r="15" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="20">
+      <c r="M14" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="N14" s="36">
+        <v>3</v>
+      </c>
+      <c r="O14" s="17"/>
+      <c r="T14" s="13"/>
+      <c r="U14" s="13"/>
+      <c r="V14" s="14"/>
+    </row>
+    <row r="15" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="21">
         <v>9</v>
       </c>
-      <c r="B15" s="20">
+      <c r="B15" s="21">
         <v>1</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="E15" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="F15" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="G15" s="14" t="s">
+      <c r="H15" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="H15" s="14" t="s">
+      <c r="I15" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="I15" s="22" t="s">
+      <c r="J15" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="J15">
+      <c r="K15" s="23">
         <v>1</v>
       </c>
-      <c r="K15" s="4">
+      <c r="L15" s="27">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="M15" s="19"/>
-      <c r="N15" s="19"/>
-      <c r="S15" s="14"/>
-      <c r="T15" s="14"/>
-      <c r="U15" s="15"/>
-    </row>
-    <row r="16" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="20">
+      <c r="M15" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="N15" s="36">
+        <v>2</v>
+      </c>
+      <c r="O15" s="17"/>
+      <c r="T15" s="13"/>
+      <c r="U15" s="13"/>
+      <c r="V15" s="14"/>
+    </row>
+    <row r="16" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="21">
         <v>10</v>
       </c>
-      <c r="B16" s="20">
+      <c r="B16" s="21">
         <v>1</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="E16" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="F16" s="30" t="s">
         <v>157</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="G16" s="14" t="s">
+      <c r="H16" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="H16" s="14" t="s">
+      <c r="I16" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="I16" s="22" t="s">
+      <c r="J16" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="J16">
+      <c r="K16" s="23">
         <v>0.12</v>
       </c>
-      <c r="K16" s="4">
+      <c r="L16" s="27">
         <f t="shared" si="1"/>
         <v>0.12</v>
       </c>
-      <c r="M16" s="19"/>
-      <c r="N16" s="19"/>
-      <c r="S16" s="14"/>
-      <c r="T16" s="14"/>
-      <c r="U16" s="15"/>
-    </row>
-    <row r="17" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="20">
+      <c r="M16" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="N16" s="36"/>
+      <c r="O16" s="17"/>
+      <c r="T16" s="13"/>
+      <c r="U16" s="13"/>
+      <c r="V16" s="14"/>
+    </row>
+    <row r="17" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="21">
         <v>11</v>
       </c>
-      <c r="B17" s="20">
+      <c r="B17" s="21">
         <v>1</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="23"/>
+      <c r="E17" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="F17" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="H17" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="H17" s="14" t="s">
+      <c r="I17" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="I17" s="22">
+      <c r="J17" s="29">
         <v>2900</v>
       </c>
-      <c r="J17">
+      <c r="K17" s="23">
         <v>14.95</v>
       </c>
-      <c r="K17" s="4">
+      <c r="L17" s="27">
         <f t="shared" si="1"/>
         <v>14.95</v>
       </c>
-      <c r="M17" s="19"/>
-      <c r="N17" s="19"/>
-      <c r="S17" s="14"/>
-      <c r="T17" s="14"/>
-      <c r="U17" s="15"/>
-    </row>
-    <row r="18" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="20">
+      <c r="M17" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="N17" s="36">
+        <v>3</v>
+      </c>
+      <c r="O17" s="17"/>
+      <c r="T17" s="13"/>
+      <c r="U17" s="13"/>
+      <c r="V17" s="14"/>
+    </row>
+    <row r="18" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="21">
         <v>12</v>
       </c>
-      <c r="B18" s="20">
+      <c r="B18" s="21">
         <v>1</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="23"/>
+      <c r="E18" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="F18" s="30" t="s">
         <v>158</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="G18" s="14" t="s">
+      <c r="H18" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="H18" s="14" t="s">
+      <c r="I18" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="I18" s="22" t="s">
+      <c r="J18" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="J18">
+      <c r="K18" s="23">
         <v>1.55</v>
       </c>
-      <c r="K18" s="4">
+      <c r="L18" s="27">
         <f t="shared" si="1"/>
         <v>1.55</v>
       </c>
-      <c r="M18" s="19"/>
-      <c r="N18" s="19"/>
-      <c r="S18" s="14"/>
-      <c r="T18" s="14"/>
-      <c r="U18" s="15"/>
-    </row>
-    <row r="19" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="20">
+      <c r="M18" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="N18" s="36">
+        <v>5</v>
+      </c>
+      <c r="O18" s="17"/>
+      <c r="T18" s="13"/>
+      <c r="U18" s="13"/>
+      <c r="V18" s="14"/>
+    </row>
+    <row r="19" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="21">
         <v>13</v>
       </c>
-      <c r="B19" s="20">
+      <c r="B19" s="21">
         <v>1</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="23"/>
+      <c r="E19" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="F19" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="G19" s="14" t="s">
+      <c r="H19" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="H19" s="14" t="s">
+      <c r="I19" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="I19" s="22">
+      <c r="J19" s="29">
         <v>27899</v>
       </c>
-      <c r="J19">
+      <c r="K19" s="23">
         <v>9.9499999999999993</v>
       </c>
-      <c r="K19" s="4">
+      <c r="L19" s="27">
         <f t="shared" si="1"/>
         <v>9.9499999999999993</v>
       </c>
-      <c r="M19" s="19"/>
-      <c r="N19" s="19"/>
-      <c r="S19" s="14"/>
-      <c r="T19" s="14"/>
-      <c r="U19" s="15"/>
-    </row>
-    <row r="20" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="20">
+      <c r="M19" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="N19" s="36">
+        <v>2</v>
+      </c>
+      <c r="O19" s="17"/>
+      <c r="T19" s="13"/>
+      <c r="U19" s="13"/>
+      <c r="V19" s="14"/>
+    </row>
+    <row r="20" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="21">
         <v>14</v>
       </c>
-      <c r="B20" s="20">
+      <c r="B20" s="21">
         <v>14</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="E20" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="F20" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="H20" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="H20" s="14" t="s">
+      <c r="I20" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="I20" s="22" t="s">
+      <c r="J20" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="J20">
+      <c r="K20" s="23">
         <v>0.1</v>
       </c>
-      <c r="K20" s="4">
+      <c r="L20" s="27">
         <f t="shared" si="1"/>
         <v>1.4000000000000001</v>
       </c>
-      <c r="M20" s="19"/>
-      <c r="N20" s="19"/>
-      <c r="S20" s="14"/>
-      <c r="T20" s="14"/>
-      <c r="U20" s="15"/>
-    </row>
-    <row r="21" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="20">
+      <c r="M20" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="N20" s="36"/>
+      <c r="O20" s="17"/>
+      <c r="T20" s="13"/>
+      <c r="U20" s="13"/>
+      <c r="V20" s="14"/>
+    </row>
+    <row r="21" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="21">
         <v>15</v>
       </c>
-      <c r="B21" s="20">
+      <c r="B21" s="21">
         <v>1</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="E21" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="F21" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="G21" s="14" t="s">
+      <c r="H21" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="H21" s="14" t="s">
+      <c r="I21" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="I21" s="22" t="s">
+      <c r="J21" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="J21">
+      <c r="K21" s="23">
         <v>0.39</v>
       </c>
-      <c r="K21" s="4">
+      <c r="L21" s="27">
         <f t="shared" si="1"/>
         <v>0.39</v>
       </c>
-      <c r="M21" s="19"/>
-      <c r="N21" s="19"/>
-      <c r="S21" s="14"/>
-      <c r="T21" s="14"/>
-      <c r="U21" s="15"/>
-    </row>
-    <row r="22" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="20">
+      <c r="M21" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="N21" s="36"/>
+      <c r="O21" s="17"/>
+      <c r="T21" s="13"/>
+      <c r="U21" s="13"/>
+      <c r="V21" s="14"/>
+    </row>
+    <row r="22" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="21">
         <v>16</v>
       </c>
-      <c r="B22" s="20">
+      <c r="B22" s="21">
         <v>2</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="E22" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="F22" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="G22" s="14" t="s">
+      <c r="H22" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="H22" s="14" t="s">
+      <c r="I22" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="I22" s="22" t="s">
+      <c r="J22" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="J22">
+      <c r="K22" s="23">
         <v>0.39</v>
       </c>
-      <c r="K22" s="4">
+      <c r="L22" s="27">
         <f t="shared" si="1"/>
         <v>0.78</v>
       </c>
-      <c r="M22" s="19"/>
-      <c r="N22" s="19"/>
-      <c r="S22" s="14"/>
-      <c r="T22" s="14"/>
-      <c r="U22" s="15"/>
-    </row>
-    <row r="23" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="20">
+      <c r="M22" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="N22" s="36"/>
+      <c r="O22" s="17"/>
+      <c r="T22" s="13"/>
+      <c r="U22" s="13"/>
+      <c r="V22" s="14"/>
+    </row>
+    <row r="23" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="21">
         <v>17</v>
       </c>
-      <c r="B23" s="20">
+      <c r="B23" s="21">
         <v>2</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="E23" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E23" s="14" t="s">
+      <c r="F23" s="30" t="s">
         <v>159</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="G23" s="14" t="s">
+      <c r="H23" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="H23" s="14" t="s">
+      <c r="I23" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="I23" s="22" t="s">
+      <c r="J23" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="J23">
+      <c r="K23" s="23">
         <v>0.1</v>
       </c>
-      <c r="K23" s="4">
+      <c r="L23" s="27">
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
-      <c r="M23" s="19"/>
-      <c r="N23" s="19"/>
-      <c r="S23" s="14"/>
-      <c r="T23" s="14"/>
-      <c r="U23" s="15"/>
-    </row>
-    <row r="24" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="20">
+      <c r="M23" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="N23" s="36"/>
+      <c r="O23" s="17"/>
+      <c r="T23" s="13"/>
+      <c r="U23" s="13"/>
+      <c r="V23" s="14"/>
+    </row>
+    <row r="24" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="21">
         <v>18</v>
       </c>
-      <c r="B24" s="20">
+      <c r="B24" s="21">
         <v>1</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="E24" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="G24" s="14" t="s">
+      <c r="H24" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="H24" s="14" t="s">
+      <c r="I24" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="I24" s="23" t="s">
+      <c r="J24" s="32" t="s">
         <v>115</v>
       </c>
-      <c r="J24">
+      <c r="K24" s="23">
         <v>0.1</v>
       </c>
-      <c r="K24" s="4">
+      <c r="L24" s="27">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="M24" s="19"/>
-      <c r="N24" s="19"/>
-      <c r="S24" s="14"/>
-      <c r="T24" s="14"/>
-      <c r="U24" s="17"/>
-    </row>
-    <row r="25" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="20">
+      <c r="M24" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="N24" s="36"/>
+      <c r="O24" s="17"/>
+      <c r="T24" s="13"/>
+      <c r="U24" s="13"/>
+      <c r="V24" s="16"/>
+    </row>
+    <row r="25" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="21">
         <v>19</v>
       </c>
-      <c r="B25" s="20">
+      <c r="B25" s="21">
         <v>5</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="E25" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="G25" s="14" t="s">
+      <c r="H25" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="H25" s="14" t="s">
+      <c r="I25" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="I25" s="22" t="s">
+      <c r="J25" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="J25">
+      <c r="K25" s="23">
         <v>0.1</v>
       </c>
-      <c r="K25" s="4">
+      <c r="L25" s="27">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="M25" s="19"/>
-      <c r="N25" s="19"/>
-      <c r="S25" s="14"/>
-      <c r="T25" s="14"/>
-      <c r="U25" s="15"/>
-    </row>
-    <row r="26" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="20">
+      <c r="M25" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="N25" s="36"/>
+      <c r="O25" s="17"/>
+      <c r="T25" s="13"/>
+      <c r="U25" s="13"/>
+      <c r="V25" s="14"/>
+    </row>
+    <row r="26" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="21">
         <v>20</v>
       </c>
-      <c r="B26" s="20">
+      <c r="B26" s="21">
         <v>1</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="E26" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="G26" s="14" t="s">
+      <c r="H26" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="H26" s="14" t="s">
+      <c r="I26" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="I26" s="22" t="s">
+      <c r="J26" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="J26">
+      <c r="K26" s="23">
         <v>0.1</v>
       </c>
-      <c r="K26" s="4">
+      <c r="L26" s="27">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="M26" s="19"/>
-      <c r="N26" s="19"/>
-      <c r="S26" s="14"/>
-      <c r="T26" s="14"/>
-      <c r="U26" s="15"/>
-    </row>
-    <row r="27" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="20">
+      <c r="M26" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="N26" s="36"/>
+      <c r="O26" s="17"/>
+      <c r="T26" s="13"/>
+      <c r="U26" s="13"/>
+      <c r="V26" s="14"/>
+    </row>
+    <row r="27" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="21">
         <v>21</v>
       </c>
-      <c r="B27" s="20">
+      <c r="B27" s="21">
         <v>1</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="E27" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="H27" s="30" t="s">
         <v>128</v>
       </c>
-      <c r="H27" s="14" t="s">
+      <c r="I27" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="I27" s="22" t="s">
+      <c r="J27" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="J27">
+      <c r="K27" s="23">
         <v>3.36</v>
       </c>
-      <c r="K27" s="4">
+      <c r="L27" s="27">
         <f t="shared" si="1"/>
         <v>3.36</v>
       </c>
-      <c r="M27" s="19"/>
-      <c r="N27" s="19"/>
-      <c r="S27" s="14"/>
-      <c r="T27" s="14"/>
-      <c r="U27" s="15"/>
-    </row>
-    <row r="28" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="20">
+      <c r="M27" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="N27" s="36"/>
+      <c r="O27" s="17"/>
+      <c r="T27" s="13"/>
+      <c r="U27" s="13"/>
+      <c r="V27" s="14"/>
+    </row>
+    <row r="28" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="21">
         <v>22</v>
       </c>
-      <c r="B28" s="20">
+      <c r="B28" s="21">
         <v>1</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="E28" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E28" s="14" t="s">
+      <c r="F28" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="G28" s="14" t="s">
+      <c r="H28" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="H28" s="14" t="s">
+      <c r="I28" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="I28" s="22" t="s">
+      <c r="J28" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="J28">
+      <c r="K28" s="23">
         <v>0.1</v>
       </c>
-      <c r="K28" s="4">
+      <c r="L28" s="27">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="M28" s="19"/>
-      <c r="N28" s="19"/>
-      <c r="Q28" s="14"/>
-      <c r="S28" s="14"/>
-      <c r="T28" s="14"/>
-      <c r="U28" s="15"/>
-    </row>
-    <row r="29" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="20">
+      <c r="M28" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="N28" s="36"/>
+      <c r="O28" s="17"/>
+      <c r="R28" s="13"/>
+      <c r="T28" s="13"/>
+      <c r="U28" s="13"/>
+      <c r="V28" s="14"/>
+    </row>
+    <row r="29" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="21">
         <v>23</v>
       </c>
-      <c r="B29" s="20">
+      <c r="B29" s="21">
         <v>1</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="23"/>
+      <c r="E29" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E29" s="14" t="s">
+      <c r="F29" s="30" t="s">
         <v>131</v>
       </c>
-      <c r="F29" s="14" t="s">
+      <c r="G29" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="G29" s="14" t="s">
+      <c r="H29" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="H29" s="14" t="s">
+      <c r="I29" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="I29" s="22" t="s">
+      <c r="J29" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="J29">
+      <c r="K29" s="23">
         <v>0.05</v>
       </c>
-      <c r="K29" s="4">
+      <c r="L29" s="27">
         <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
-      <c r="M29" s="19"/>
-      <c r="N29" s="19"/>
-      <c r="Q29" s="14"/>
-      <c r="R29" s="14"/>
-      <c r="S29" s="14"/>
-      <c r="T29" s="14"/>
-      <c r="U29" s="15"/>
-    </row>
-    <row r="30" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="20">
+      <c r="M29" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="N29" s="36">
+        <v>5</v>
+      </c>
+      <c r="O29" s="17"/>
+      <c r="R29" s="13"/>
+      <c r="S29" s="13"/>
+      <c r="T29" s="13"/>
+      <c r="U29" s="13"/>
+      <c r="V29" s="14"/>
+    </row>
+    <row r="30" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="21">
         <v>24</v>
       </c>
-      <c r="B30" s="20">
+      <c r="B30" s="21">
         <v>1</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="23"/>
+      <c r="E30" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E30" s="14" t="s">
+      <c r="F30" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="G30" s="14" t="s">
+      <c r="H30" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="H30" s="14" t="s">
+      <c r="I30" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="I30" s="22" t="s">
+      <c r="J30" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="J30">
+      <c r="K30" s="23">
         <v>7.76</v>
       </c>
-      <c r="K30" s="4">
+      <c r="L30" s="27">
         <f t="shared" si="1"/>
         <v>7.76</v>
       </c>
-      <c r="M30" s="19"/>
-      <c r="N30" s="19"/>
-      <c r="Q30" s="14"/>
-      <c r="S30" s="14"/>
-      <c r="T30" s="14"/>
-      <c r="U30" s="15"/>
-    </row>
-    <row r="31" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="20">
+      <c r="M30" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="N30" s="36">
+        <v>100</v>
+      </c>
+      <c r="O30" s="17"/>
+      <c r="R30" s="13"/>
+      <c r="T30" s="13"/>
+      <c r="U30" s="13"/>
+      <c r="V30" s="14"/>
+    </row>
+    <row r="31" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="21">
         <v>25</v>
       </c>
-      <c r="B31" s="20">
+      <c r="B31" s="21">
         <v>1</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="23"/>
+      <c r="E31" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E31" s="14" t="s">
+      <c r="F31" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="F31" s="14" t="s">
+      <c r="G31" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="G31" s="14" t="s">
+      <c r="H31" s="30" t="s">
         <v>139</v>
       </c>
-      <c r="H31" s="14" t="s">
+      <c r="I31" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="I31" s="22">
+      <c r="J31" s="29">
         <v>3405</v>
       </c>
-      <c r="J31">
+      <c r="K31" s="23">
         <v>19.95</v>
       </c>
-      <c r="K31" s="4">
+      <c r="L31" s="27">
         <f t="shared" si="1"/>
         <v>19.95</v>
       </c>
-      <c r="M31" s="19"/>
-      <c r="N31" s="19"/>
-      <c r="Q31" s="14"/>
-      <c r="R31" s="14"/>
-      <c r="S31" s="14"/>
-      <c r="T31" s="14"/>
-      <c r="U31" s="15"/>
-    </row>
-    <row r="32" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="20">
+      <c r="M31" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="N31" s="36">
+        <v>2</v>
+      </c>
+      <c r="O31" s="17"/>
+      <c r="R31" s="13"/>
+      <c r="S31" s="13"/>
+      <c r="T31" s="13"/>
+      <c r="U31" s="13"/>
+      <c r="V31" s="14"/>
+    </row>
+    <row r="32" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="21">
         <v>26</v>
       </c>
-      <c r="B32" s="20">
+      <c r="B32" s="21">
         <v>1</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="23"/>
+      <c r="E32" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E32" s="14" t="s">
+      <c r="F32" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="F32" s="14" t="s">
+      <c r="G32" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="G32" s="14" t="s">
+      <c r="H32" s="30" t="s">
         <v>140</v>
       </c>
-      <c r="H32" s="14" t="s">
+      <c r="I32" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="I32" s="22">
+      <c r="J32" s="29">
         <v>385</v>
       </c>
-      <c r="J32">
+      <c r="K32" s="23">
         <v>9.9499999999999993</v>
       </c>
-      <c r="K32" s="4">
+      <c r="L32" s="27">
         <f t="shared" si="1"/>
         <v>9.9499999999999993</v>
       </c>
-      <c r="M32" s="19"/>
-      <c r="N32" s="19"/>
-      <c r="Q32" s="14"/>
-      <c r="R32" s="14"/>
-      <c r="S32" s="14"/>
-      <c r="T32" s="14"/>
-      <c r="U32" s="15"/>
-    </row>
-    <row r="33" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="20">
+      <c r="M32" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="N32" s="36">
+        <v>2</v>
+      </c>
+      <c r="O32" s="17"/>
+      <c r="R32" s="13"/>
+      <c r="S32" s="13"/>
+      <c r="T32" s="13"/>
+      <c r="U32" s="13"/>
+      <c r="V32" s="14"/>
+    </row>
+    <row r="33" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="21">
         <v>27</v>
       </c>
-      <c r="B33" s="20">
+      <c r="B33" s="21">
         <v>1</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="23"/>
+      <c r="E33" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E33" s="14" t="s">
+      <c r="F33" s="30" t="s">
         <v>144</v>
       </c>
-      <c r="F33" s="14" t="s">
+      <c r="G33" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="G33" s="14" t="s">
+      <c r="H33" s="30" t="s">
         <v>143</v>
       </c>
-      <c r="H33" s="14" t="s">
+      <c r="I33" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="I33" s="24" t="s">
+      <c r="J33" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="J33">
+      <c r="K33" s="23">
         <v>2.2000000000000002</v>
       </c>
-      <c r="K33" s="4">
+      <c r="L33" s="27">
         <f t="shared" si="1"/>
         <v>2.2000000000000002</v>
       </c>
-      <c r="M33" s="19"/>
-      <c r="N33" s="19"/>
-      <c r="Q33" s="14"/>
-      <c r="R33" s="14"/>
-      <c r="S33" s="14"/>
-      <c r="T33" s="14"/>
-      <c r="U33" s="14"/>
-    </row>
-    <row r="34" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="20">
+      <c r="M33" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="N33" s="36">
+        <v>4</v>
+      </c>
+      <c r="O33" s="17"/>
+      <c r="R33" s="13"/>
+      <c r="S33" s="13"/>
+      <c r="T33" s="13"/>
+      <c r="U33" s="13"/>
+      <c r="V33" s="13"/>
+    </row>
+    <row r="34" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="21">
         <v>28</v>
       </c>
-      <c r="B34" s="20">
+      <c r="B34" s="21">
         <v>1</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="23"/>
+      <c r="E34" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E34" s="14" t="s">
+      <c r="F34" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="F34" s="14" t="s">
+      <c r="G34" s="30" t="s">
         <v>145</v>
       </c>
-      <c r="G34" s="14" t="s">
+      <c r="H34" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="H34" s="14" t="s">
+      <c r="I34" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="I34" s="22">
+      <c r="J34" s="29">
         <v>4918</v>
       </c>
-      <c r="J34">
+      <c r="K34" s="23">
         <v>5.95</v>
       </c>
-      <c r="K34" s="4">
+      <c r="L34" s="27">
         <f t="shared" si="1"/>
         <v>5.95</v>
       </c>
-      <c r="M34" s="19"/>
-      <c r="N34" s="19"/>
-      <c r="Q34" s="14"/>
-      <c r="R34" s="14"/>
-      <c r="S34" s="14"/>
-      <c r="T34" s="14"/>
-      <c r="U34" s="15"/>
-    </row>
-    <row r="35" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="20">
+      <c r="M34" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="N34" s="36">
+        <v>3</v>
+      </c>
+      <c r="O34" s="17"/>
+      <c r="R34" s="13"/>
+      <c r="S34" s="13"/>
+      <c r="T34" s="13"/>
+      <c r="U34" s="13"/>
+      <c r="V34" s="14"/>
+    </row>
+    <row r="35" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="21">
         <v>29</v>
       </c>
-      <c r="B35" s="20">
+      <c r="B35" s="21">
         <v>1</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="23"/>
+      <c r="E35" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E35" s="14" t="s">
+      <c r="F35" s="30" t="s">
         <v>147</v>
       </c>
-      <c r="F35" s="14" t="s">
+      <c r="G35" s="30" t="s">
         <v>148</v>
       </c>
-      <c r="G35" s="14" t="s">
+      <c r="H35" s="30" t="s">
         <v>149</v>
       </c>
-      <c r="H35" s="14" t="s">
+      <c r="I35" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="I35" s="22" t="s">
+      <c r="J35" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="J35">
+      <c r="K35" s="23">
         <v>2.2999999999999998</v>
       </c>
-      <c r="K35" s="4">
+      <c r="L35" s="27">
         <f t="shared" si="1"/>
         <v>2.2999999999999998</v>
       </c>
-      <c r="M35" s="19"/>
-      <c r="N35" s="19"/>
-      <c r="Q35" s="14"/>
-      <c r="R35" s="14"/>
-      <c r="S35" s="14"/>
-      <c r="T35" s="14"/>
-      <c r="U35" s="15"/>
-    </row>
-    <row r="36" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="20">
+      <c r="M35" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="N35" s="36">
+        <v>1</v>
+      </c>
+      <c r="O35" s="17"/>
+      <c r="R35" s="13"/>
+      <c r="S35" s="13"/>
+      <c r="T35" s="13"/>
+      <c r="U35" s="13"/>
+      <c r="V35" s="14"/>
+    </row>
+    <row r="36" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="21">
         <v>30</v>
       </c>
-      <c r="B36" s="20">
+      <c r="B36" s="21">
         <v>1</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="23"/>
+      <c r="E36" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E36" s="14" t="s">
+      <c r="F36" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="G36" s="14" t="s">
+      <c r="H36" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="H36" s="14" t="s">
+      <c r="I36" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="I36" s="23" t="s">
+      <c r="J36" s="32" t="s">
         <v>152</v>
       </c>
-      <c r="J36" s="18">
+      <c r="K36" s="30">
         <v>6.29</v>
       </c>
-      <c r="K36" s="4">
+      <c r="L36" s="27">
         <f t="shared" si="1"/>
         <v>6.29</v>
       </c>
-      <c r="M36" s="19"/>
-      <c r="N36" s="19"/>
-      <c r="Q36" s="14"/>
-      <c r="S36" s="14"/>
-      <c r="T36" s="14"/>
-      <c r="U36" s="17"/>
-      <c r="V36" s="18"/>
-      <c r="AC36" s="15"/>
-    </row>
-    <row r="37" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="20"/>
-      <c r="B37" s="20"/>
-    </row>
-    <row r="38" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="20"/>
-      <c r="B38" s="20"/>
-    </row>
-    <row r="39" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="20"/>
-      <c r="B39" s="20"/>
-      <c r="J39" s="9" t="s">
+      <c r="M36" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="N36" s="36">
+        <v>5</v>
+      </c>
+      <c r="O36" s="17"/>
+      <c r="R36" s="13"/>
+      <c r="T36" s="13"/>
+      <c r="U36" s="13"/>
+      <c r="V36" s="16"/>
+      <c r="W36" s="13"/>
+      <c r="AD36" s="14"/>
+    </row>
+    <row r="37" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="18"/>
+      <c r="B37" s="18"/>
+    </row>
+    <row r="38" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="18"/>
+      <c r="B38" s="18"/>
+    </row>
+    <row r="39" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="18"/>
+      <c r="B39" s="18"/>
+      <c r="K39" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="K39" s="9">
-        <f>SUM(K7:K36)</f>
+      <c r="L39" s="9">
+        <f>SUM(L7:L36)</f>
         <v>98.480000000000018</v>
       </c>
     </row>
-    <row r="40" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
         <v>41</v>
       </c>
@@ -2255,14 +2800,15 @@
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
       <c r="I40" s="6"/>
-      <c r="J40" s="7"/>
+      <c r="J40" s="6"/>
       <c r="K40" s="7"/>
-    </row>
-    <row r="41" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J41" s="4"/>
+      <c r="L40" s="7"/>
+    </row>
+    <row r="41" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K41" s="4"/>
-    </row>
-    <row r="42" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L41" s="4"/>
+    </row>
+    <row r="42" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="10" t="s">
         <v>42</v>
       </c>
@@ -2270,13 +2816,14 @@
       <c r="C42" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D42" s="10" t="s">
+      <c r="D42" s="11"/>
+      <c r="E42" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J42" s="4"/>
       <c r="K42" s="4"/>
-    </row>
-    <row r="43" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L42" s="4"/>
+    </row>
+    <row r="43" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>45</v>
       </c>
@@ -2284,785 +2831,809 @@
       <c r="C43" s="12">
         <v>45237</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D43" s="12"/>
+      <c r="E43" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="J43" s="4"/>
       <c r="K43" s="4"/>
-    </row>
-    <row r="44" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="16" t="s">
+      <c r="L43" s="4"/>
+    </row>
+    <row r="44" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="15" t="s">
         <v>153</v>
       </c>
       <c r="C44" s="12">
         <v>45243</v>
       </c>
-      <c r="D44" s="14" t="s">
+      <c r="D44" s="12"/>
+      <c r="E44" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="J44" s="4"/>
       <c r="K44" s="4"/>
-    </row>
-    <row r="45" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J45" s="4"/>
+      <c r="L44" s="4"/>
+    </row>
+    <row r="45" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>160</v>
+      </c>
+      <c r="C45" s="12">
+        <v>45252</v>
+      </c>
+      <c r="E45" t="s">
+        <v>161</v>
+      </c>
       <c r="K45" s="4"/>
-    </row>
-    <row r="46" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J46" s="4"/>
+      <c r="L45" s="4"/>
+    </row>
+    <row r="46" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C46" s="12"/>
       <c r="K46" s="4"/>
-    </row>
-    <row r="47" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J47" s="4"/>
+      <c r="L46" s="4"/>
+    </row>
+    <row r="47" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C47" s="12"/>
       <c r="K47" s="4"/>
-    </row>
-    <row r="48" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J48" s="4"/>
+      <c r="L47" s="4"/>
+    </row>
+    <row r="48" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C48" s="12"/>
       <c r="K48" s="4"/>
-    </row>
-    <row r="49" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J49" s="4"/>
+      <c r="L48" s="4"/>
+    </row>
+    <row r="49" spans="3:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C49" s="12"/>
       <c r="K49" s="4"/>
-    </row>
-    <row r="50" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J50" s="4"/>
+      <c r="L49" s="4"/>
+    </row>
+    <row r="50" spans="3:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C50" s="12"/>
       <c r="K50" s="4"/>
-    </row>
-    <row r="51" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J51" s="4"/>
+      <c r="L50" s="4"/>
+    </row>
+    <row r="51" spans="3:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C51" s="12"/>
       <c r="K51" s="4"/>
-    </row>
-    <row r="52" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J52" s="4"/>
+      <c r="L51" s="4"/>
+    </row>
+    <row r="52" spans="3:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C52" s="12"/>
       <c r="K52" s="4"/>
-    </row>
-    <row r="53" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J53" s="4"/>
+      <c r="L52" s="4"/>
+    </row>
+    <row r="53" spans="3:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C53" s="12"/>
       <c r="K53" s="4"/>
-    </row>
-    <row r="54" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J54" s="4"/>
+      <c r="L53" s="4"/>
+    </row>
+    <row r="54" spans="3:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C54" s="12"/>
       <c r="K54" s="4"/>
-    </row>
-    <row r="55" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J55" s="4"/>
+      <c r="L54" s="4"/>
+    </row>
+    <row r="55" spans="3:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C55" s="12"/>
       <c r="K55" s="4"/>
-    </row>
-    <row r="56" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J56" s="4"/>
+      <c r="L55" s="4"/>
+    </row>
+    <row r="56" spans="3:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C56" s="12"/>
       <c r="K56" s="4"/>
-    </row>
-    <row r="57" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J57" s="4"/>
+      <c r="L56" s="4"/>
+    </row>
+    <row r="57" spans="3:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C57" s="12"/>
       <c r="K57" s="4"/>
-    </row>
-    <row r="58" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J58" s="4"/>
+      <c r="L57" s="4"/>
+    </row>
+    <row r="58" spans="3:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C58" s="12"/>
       <c r="K58" s="4"/>
-    </row>
-    <row r="59" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J59" s="4"/>
+      <c r="L58" s="4"/>
+    </row>
+    <row r="59" spans="3:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K59" s="4"/>
-    </row>
-    <row r="60" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J60" s="4"/>
+      <c r="L59" s="4"/>
+    </row>
+    <row r="60" spans="3:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K60" s="4"/>
-    </row>
-    <row r="61" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J61" s="4"/>
+      <c r="L60" s="4"/>
+    </row>
+    <row r="61" spans="3:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K61" s="4"/>
-    </row>
-    <row r="62" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J62" s="4"/>
+      <c r="L61" s="4"/>
+    </row>
+    <row r="62" spans="3:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K62" s="4"/>
-    </row>
-    <row r="63" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J63" s="4"/>
+      <c r="L62" s="4"/>
+    </row>
+    <row r="63" spans="3:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K63" s="4"/>
-    </row>
-    <row r="64" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J64" s="4"/>
+      <c r="L63" s="4"/>
+    </row>
+    <row r="64" spans="3:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K64" s="4"/>
-    </row>
-    <row r="65" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J65" s="4"/>
+      <c r="L64" s="4"/>
+    </row>
+    <row r="65" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K65" s="4"/>
-    </row>
-    <row r="66" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J66" s="4"/>
+      <c r="L65" s="4"/>
+    </row>
+    <row r="66" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K66" s="4"/>
-    </row>
-    <row r="67" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J67" s="4"/>
+      <c r="L66" s="4"/>
+    </row>
+    <row r="67" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K67" s="4"/>
-    </row>
-    <row r="68" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J68" s="4"/>
+      <c r="L67" s="4"/>
+    </row>
+    <row r="68" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K68" s="4"/>
-    </row>
-    <row r="69" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J69" s="4"/>
+      <c r="L68" s="4"/>
+    </row>
+    <row r="69" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K69" s="4"/>
-    </row>
-    <row r="70" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J70" s="4"/>
+      <c r="L69" s="4"/>
+    </row>
+    <row r="70" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K70" s="4"/>
-    </row>
-    <row r="71" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J71" s="4"/>
+      <c r="L70" s="4"/>
+    </row>
+    <row r="71" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K71" s="4"/>
-    </row>
-    <row r="72" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J72" s="4"/>
+      <c r="L71" s="4"/>
+    </row>
+    <row r="72" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K72" s="4"/>
-    </row>
-    <row r="73" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J73" s="4"/>
+      <c r="L72" s="4"/>
+    </row>
+    <row r="73" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K73" s="4"/>
-    </row>
-    <row r="74" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J74" s="4"/>
+      <c r="L73" s="4"/>
+    </row>
+    <row r="74" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K74" s="4"/>
-    </row>
-    <row r="75" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J75" s="4"/>
+      <c r="L74" s="4"/>
+    </row>
+    <row r="75" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K75" s="4"/>
-    </row>
-    <row r="76" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J76" s="4"/>
+      <c r="L75" s="4"/>
+    </row>
+    <row r="76" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K76" s="4"/>
-    </row>
-    <row r="77" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J77" s="4"/>
+      <c r="L76" s="4"/>
+    </row>
+    <row r="77" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K77" s="4"/>
-    </row>
-    <row r="78" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J78" s="4"/>
+      <c r="L77" s="4"/>
+    </row>
+    <row r="78" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K78" s="4"/>
-    </row>
-    <row r="79" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J79" s="4"/>
+      <c r="L78" s="4"/>
+    </row>
+    <row r="79" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K79" s="4"/>
-    </row>
-    <row r="80" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J80" s="4"/>
+      <c r="L79" s="4"/>
+    </row>
+    <row r="80" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K80" s="4"/>
-    </row>
-    <row r="81" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J81" s="4"/>
+      <c r="L80" s="4"/>
+    </row>
+    <row r="81" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K81" s="4"/>
-    </row>
-    <row r="82" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J82" s="4"/>
+      <c r="L81" s="4"/>
+    </row>
+    <row r="82" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K82" s="4"/>
-    </row>
-    <row r="83" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J83" s="4"/>
+      <c r="L82" s="4"/>
+    </row>
+    <row r="83" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K83" s="4"/>
-    </row>
-    <row r="84" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J84" s="4"/>
+      <c r="L83" s="4"/>
+    </row>
+    <row r="84" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K84" s="4"/>
-    </row>
-    <row r="85" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J85" s="4"/>
+      <c r="L84" s="4"/>
+    </row>
+    <row r="85" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K85" s="4"/>
-    </row>
-    <row r="86" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J86" s="4"/>
+      <c r="L85" s="4"/>
+    </row>
+    <row r="86" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K86" s="4"/>
-    </row>
-    <row r="87" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J87" s="4"/>
+      <c r="L86" s="4"/>
+    </row>
+    <row r="87" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K87" s="4"/>
-    </row>
-    <row r="88" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J88" s="4"/>
+      <c r="L87" s="4"/>
+    </row>
+    <row r="88" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K88" s="4"/>
-    </row>
-    <row r="89" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J89" s="4"/>
+      <c r="L88" s="4"/>
+    </row>
+    <row r="89" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K89" s="4"/>
-    </row>
-    <row r="90" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J90" s="4"/>
+      <c r="L89" s="4"/>
+    </row>
+    <row r="90" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K90" s="4"/>
-    </row>
-    <row r="91" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J91" s="4"/>
+      <c r="L90" s="4"/>
+    </row>
+    <row r="91" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K91" s="4"/>
-    </row>
-    <row r="92" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J92" s="4"/>
+      <c r="L91" s="4"/>
+    </row>
+    <row r="92" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K92" s="4"/>
-    </row>
-    <row r="93" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J93" s="4"/>
+      <c r="L92" s="4"/>
+    </row>
+    <row r="93" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K93" s="4"/>
-    </row>
-    <row r="94" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J94" s="4"/>
+      <c r="L93" s="4"/>
+    </row>
+    <row r="94" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K94" s="4"/>
-    </row>
-    <row r="95" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J95" s="4"/>
+      <c r="L94" s="4"/>
+    </row>
+    <row r="95" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K95" s="4"/>
-    </row>
-    <row r="96" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J96" s="4"/>
+      <c r="L95" s="4"/>
+    </row>
+    <row r="96" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K96" s="4"/>
-    </row>
-    <row r="97" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J97" s="4"/>
+      <c r="L96" s="4"/>
+    </row>
+    <row r="97" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K97" s="4"/>
-    </row>
-    <row r="98" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J98" s="4"/>
+      <c r="L97" s="4"/>
+    </row>
+    <row r="98" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K98" s="4"/>
-    </row>
-    <row r="99" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J99" s="4"/>
+      <c r="L98" s="4"/>
+    </row>
+    <row r="99" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K99" s="4"/>
-    </row>
-    <row r="100" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J100" s="4"/>
+      <c r="L99" s="4"/>
+    </row>
+    <row r="100" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K100" s="4"/>
-    </row>
-    <row r="101" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J101" s="4"/>
+      <c r="L100" s="4"/>
+    </row>
+    <row r="101" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K101" s="4"/>
-    </row>
-    <row r="102" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J102" s="4"/>
+      <c r="L101" s="4"/>
+    </row>
+    <row r="102" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K102" s="4"/>
-    </row>
-    <row r="103" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J103" s="4"/>
+      <c r="L102" s="4"/>
+    </row>
+    <row r="103" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K103" s="4"/>
-    </row>
-    <row r="104" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J104" s="4"/>
+      <c r="L103" s="4"/>
+    </row>
+    <row r="104" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K104" s="4"/>
-    </row>
-    <row r="105" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J105" s="4"/>
+      <c r="L104" s="4"/>
+    </row>
+    <row r="105" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K105" s="4"/>
-    </row>
-    <row r="106" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J106" s="4"/>
+      <c r="L105" s="4"/>
+    </row>
+    <row r="106" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K106" s="4"/>
-    </row>
-    <row r="107" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J107" s="4"/>
+      <c r="L106" s="4"/>
+    </row>
+    <row r="107" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K107" s="4"/>
-    </row>
-    <row r="108" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J108" s="4"/>
+      <c r="L107" s="4"/>
+    </row>
+    <row r="108" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K108" s="4"/>
-    </row>
-    <row r="109" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J109" s="4"/>
+      <c r="L108" s="4"/>
+    </row>
+    <row r="109" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K109" s="4"/>
-    </row>
-    <row r="110" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J110" s="4"/>
+      <c r="L109" s="4"/>
+    </row>
+    <row r="110" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K110" s="4"/>
-    </row>
-    <row r="111" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J111" s="4"/>
+      <c r="L110" s="4"/>
+    </row>
+    <row r="111" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K111" s="4"/>
-    </row>
-    <row r="112" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J112" s="4"/>
+      <c r="L111" s="4"/>
+    </row>
+    <row r="112" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K112" s="4"/>
-    </row>
-    <row r="113" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J113" s="4"/>
+      <c r="L112" s="4"/>
+    </row>
+    <row r="113" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K113" s="4"/>
-    </row>
-    <row r="114" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J114" s="4"/>
+      <c r="L113" s="4"/>
+    </row>
+    <row r="114" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K114" s="4"/>
-    </row>
-    <row r="115" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J115" s="4"/>
+      <c r="L114" s="4"/>
+    </row>
+    <row r="115" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K115" s="4"/>
-    </row>
-    <row r="116" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J116" s="4"/>
+      <c r="L115" s="4"/>
+    </row>
+    <row r="116" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K116" s="4"/>
-    </row>
-    <row r="117" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J117" s="4"/>
+      <c r="L116" s="4"/>
+    </row>
+    <row r="117" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K117" s="4"/>
-    </row>
-    <row r="118" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J118" s="4"/>
+      <c r="L117" s="4"/>
+    </row>
+    <row r="118" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K118" s="4"/>
-    </row>
-    <row r="119" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J119" s="4"/>
+      <c r="L118" s="4"/>
+    </row>
+    <row r="119" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K119" s="4"/>
-    </row>
-    <row r="120" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J120" s="4"/>
+      <c r="L119" s="4"/>
+    </row>
+    <row r="120" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K120" s="4"/>
-    </row>
-    <row r="121" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J121" s="4"/>
+      <c r="L120" s="4"/>
+    </row>
+    <row r="121" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K121" s="4"/>
-    </row>
-    <row r="122" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J122" s="4"/>
+      <c r="L121" s="4"/>
+    </row>
+    <row r="122" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K122" s="4"/>
-    </row>
-    <row r="123" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J123" s="4"/>
+      <c r="L122" s="4"/>
+    </row>
+    <row r="123" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K123" s="4"/>
-    </row>
-    <row r="124" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J124" s="4"/>
+      <c r="L123" s="4"/>
+    </row>
+    <row r="124" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K124" s="4"/>
-    </row>
-    <row r="125" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J125" s="4"/>
+      <c r="L124" s="4"/>
+    </row>
+    <row r="125" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K125" s="4"/>
-    </row>
-    <row r="126" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J126" s="4"/>
+      <c r="L125" s="4"/>
+    </row>
+    <row r="126" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K126" s="4"/>
-    </row>
-    <row r="127" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J127" s="4"/>
+      <c r="L126" s="4"/>
+    </row>
+    <row r="127" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K127" s="4"/>
-    </row>
-    <row r="128" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J128" s="4"/>
+      <c r="L127" s="4"/>
+    </row>
+    <row r="128" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K128" s="4"/>
-    </row>
-    <row r="129" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J129" s="4"/>
+      <c r="L128" s="4"/>
+    </row>
+    <row r="129" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K129" s="4"/>
-    </row>
-    <row r="130" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J130" s="4"/>
+      <c r="L129" s="4"/>
+    </row>
+    <row r="130" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K130" s="4"/>
-    </row>
-    <row r="131" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J131" s="4"/>
+      <c r="L130" s="4"/>
+    </row>
+    <row r="131" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K131" s="4"/>
-    </row>
-    <row r="132" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J132" s="4"/>
+      <c r="L131" s="4"/>
+    </row>
+    <row r="132" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K132" s="4"/>
-    </row>
-    <row r="133" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J133" s="4"/>
+      <c r="L132" s="4"/>
+    </row>
+    <row r="133" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K133" s="4"/>
-    </row>
-    <row r="134" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J134" s="4"/>
+      <c r="L133" s="4"/>
+    </row>
+    <row r="134" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K134" s="4"/>
-    </row>
-    <row r="135" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J135" s="4"/>
+      <c r="L134" s="4"/>
+    </row>
+    <row r="135" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K135" s="4"/>
-    </row>
-    <row r="136" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J136" s="4"/>
+      <c r="L135" s="4"/>
+    </row>
+    <row r="136" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K136" s="4"/>
-    </row>
-    <row r="137" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J137" s="4"/>
+      <c r="L136" s="4"/>
+    </row>
+    <row r="137" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K137" s="4"/>
-    </row>
-    <row r="138" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J138" s="4"/>
+      <c r="L137" s="4"/>
+    </row>
+    <row r="138" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K138" s="4"/>
-    </row>
-    <row r="139" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J139" s="4"/>
+      <c r="L138" s="4"/>
+    </row>
+    <row r="139" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K139" s="4"/>
-    </row>
-    <row r="140" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J140" s="4"/>
+      <c r="L139" s="4"/>
+    </row>
+    <row r="140" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K140" s="4"/>
-    </row>
-    <row r="141" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J141" s="4"/>
+      <c r="L140" s="4"/>
+    </row>
+    <row r="141" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K141" s="4"/>
-    </row>
-    <row r="142" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J142" s="4"/>
+      <c r="L141" s="4"/>
+    </row>
+    <row r="142" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K142" s="4"/>
-    </row>
-    <row r="143" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J143" s="4"/>
+      <c r="L142" s="4"/>
+    </row>
+    <row r="143" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K143" s="4"/>
-    </row>
-    <row r="144" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J144" s="4"/>
+      <c r="L143" s="4"/>
+    </row>
+    <row r="144" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K144" s="4"/>
-    </row>
-    <row r="145" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J145" s="4"/>
+      <c r="L144" s="4"/>
+    </row>
+    <row r="145" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K145" s="4"/>
-    </row>
-    <row r="146" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J146" s="4"/>
+      <c r="L145" s="4"/>
+    </row>
+    <row r="146" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K146" s="4"/>
-    </row>
-    <row r="147" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J147" s="4"/>
+      <c r="L146" s="4"/>
+    </row>
+    <row r="147" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K147" s="4"/>
-    </row>
-    <row r="148" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J148" s="4"/>
+      <c r="L147" s="4"/>
+    </row>
+    <row r="148" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K148" s="4"/>
-    </row>
-    <row r="149" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J149" s="4"/>
+      <c r="L148" s="4"/>
+    </row>
+    <row r="149" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K149" s="4"/>
-    </row>
-    <row r="150" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J150" s="4"/>
+      <c r="L149" s="4"/>
+    </row>
+    <row r="150" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K150" s="4"/>
-    </row>
-    <row r="151" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J151" s="4"/>
+      <c r="L150" s="4"/>
+    </row>
+    <row r="151" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K151" s="4"/>
-    </row>
-    <row r="152" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J152" s="4"/>
+      <c r="L151" s="4"/>
+    </row>
+    <row r="152" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K152" s="4"/>
-    </row>
-    <row r="153" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J153" s="4"/>
+      <c r="L152" s="4"/>
+    </row>
+    <row r="153" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K153" s="4"/>
-    </row>
-    <row r="154" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J154" s="4"/>
+      <c r="L153" s="4"/>
+    </row>
+    <row r="154" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K154" s="4"/>
-    </row>
-    <row r="155" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J155" s="4"/>
+      <c r="L154" s="4"/>
+    </row>
+    <row r="155" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K155" s="4"/>
-    </row>
-    <row r="156" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J156" s="4"/>
+      <c r="L155" s="4"/>
+    </row>
+    <row r="156" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K156" s="4"/>
-    </row>
-    <row r="157" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J157" s="4"/>
+      <c r="L156" s="4"/>
+    </row>
+    <row r="157" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K157" s="4"/>
-    </row>
-    <row r="158" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J158" s="4"/>
+      <c r="L157" s="4"/>
+    </row>
+    <row r="158" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K158" s="4"/>
-    </row>
-    <row r="159" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J159" s="4"/>
+      <c r="L158" s="4"/>
+    </row>
+    <row r="159" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K159" s="4"/>
-    </row>
-    <row r="160" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J160" s="4"/>
+      <c r="L159" s="4"/>
+    </row>
+    <row r="160" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K160" s="4"/>
-    </row>
-    <row r="161" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J161" s="4"/>
+      <c r="L160" s="4"/>
+    </row>
+    <row r="161" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K161" s="4"/>
-    </row>
-    <row r="162" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J162" s="4"/>
+      <c r="L161" s="4"/>
+    </row>
+    <row r="162" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K162" s="4"/>
-    </row>
-    <row r="163" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J163" s="4"/>
+      <c r="L162" s="4"/>
+    </row>
+    <row r="163" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K163" s="4"/>
-    </row>
-    <row r="164" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J164" s="4"/>
+      <c r="L163" s="4"/>
+    </row>
+    <row r="164" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K164" s="4"/>
-    </row>
-    <row r="165" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J165" s="4"/>
+      <c r="L164" s="4"/>
+    </row>
+    <row r="165" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K165" s="4"/>
-    </row>
-    <row r="166" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J166" s="4"/>
+      <c r="L165" s="4"/>
+    </row>
+    <row r="166" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K166" s="4"/>
-    </row>
-    <row r="167" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J167" s="4"/>
+      <c r="L166" s="4"/>
+    </row>
+    <row r="167" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K167" s="4"/>
-    </row>
-    <row r="168" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J168" s="4"/>
+      <c r="L167" s="4"/>
+    </row>
+    <row r="168" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K168" s="4"/>
-    </row>
-    <row r="169" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J169" s="4"/>
+      <c r="L168" s="4"/>
+    </row>
+    <row r="169" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K169" s="4"/>
-    </row>
-    <row r="170" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J170" s="4"/>
+      <c r="L169" s="4"/>
+    </row>
+    <row r="170" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K170" s="4"/>
-    </row>
-    <row r="171" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J171" s="4"/>
+      <c r="L170" s="4"/>
+    </row>
+    <row r="171" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K171" s="4"/>
-    </row>
-    <row r="172" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J172" s="4"/>
+      <c r="L171" s="4"/>
+    </row>
+    <row r="172" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K172" s="4"/>
-    </row>
-    <row r="173" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J173" s="4"/>
+      <c r="L172" s="4"/>
+    </row>
+    <row r="173" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K173" s="4"/>
-    </row>
-    <row r="174" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J174" s="4"/>
+      <c r="L173" s="4"/>
+    </row>
+    <row r="174" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K174" s="4"/>
-    </row>
-    <row r="175" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J175" s="4"/>
+      <c r="L174" s="4"/>
+    </row>
+    <row r="175" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K175" s="4"/>
-    </row>
-    <row r="176" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J176" s="4"/>
+      <c r="L175" s="4"/>
+    </row>
+    <row r="176" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K176" s="4"/>
-    </row>
-    <row r="177" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J177" s="4"/>
+      <c r="L176" s="4"/>
+    </row>
+    <row r="177" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K177" s="4"/>
-    </row>
-    <row r="178" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J178" s="4"/>
+      <c r="L177" s="4"/>
+    </row>
+    <row r="178" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K178" s="4"/>
-    </row>
-    <row r="179" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J179" s="4"/>
+      <c r="L178" s="4"/>
+    </row>
+    <row r="179" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K179" s="4"/>
-    </row>
-    <row r="180" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J180" s="4"/>
+      <c r="L179" s="4"/>
+    </row>
+    <row r="180" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K180" s="4"/>
-    </row>
-    <row r="181" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J181" s="4"/>
+      <c r="L180" s="4"/>
+    </row>
+    <row r="181" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K181" s="4"/>
-    </row>
-    <row r="182" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J182" s="4"/>
+      <c r="L181" s="4"/>
+    </row>
+    <row r="182" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K182" s="4"/>
-    </row>
-    <row r="183" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J183" s="4"/>
+      <c r="L182" s="4"/>
+    </row>
+    <row r="183" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K183" s="4"/>
-    </row>
-    <row r="184" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J184" s="4"/>
+      <c r="L183" s="4"/>
+    </row>
+    <row r="184" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K184" s="4"/>
-    </row>
-    <row r="185" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J185" s="4"/>
+      <c r="L184" s="4"/>
+    </row>
+    <row r="185" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K185" s="4"/>
-    </row>
-    <row r="186" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J186" s="4"/>
+      <c r="L185" s="4"/>
+    </row>
+    <row r="186" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K186" s="4"/>
-    </row>
-    <row r="187" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J187" s="4"/>
+      <c r="L186" s="4"/>
+    </row>
+    <row r="187" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K187" s="4"/>
-    </row>
-    <row r="188" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J188" s="4"/>
+      <c r="L187" s="4"/>
+    </row>
+    <row r="188" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K188" s="4"/>
-    </row>
-    <row r="189" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J189" s="4"/>
+      <c r="L188" s="4"/>
+    </row>
+    <row r="189" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K189" s="4"/>
-    </row>
-    <row r="190" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J190" s="4"/>
+      <c r="L189" s="4"/>
+    </row>
+    <row r="190" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K190" s="4"/>
-    </row>
-    <row r="191" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J191" s="4"/>
+      <c r="L190" s="4"/>
+    </row>
+    <row r="191" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K191" s="4"/>
-    </row>
-    <row r="192" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J192" s="4"/>
+      <c r="L191" s="4"/>
+    </row>
+    <row r="192" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K192" s="4"/>
-    </row>
-    <row r="193" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J193" s="4"/>
+      <c r="L192" s="4"/>
+    </row>
+    <row r="193" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K193" s="4"/>
-    </row>
-    <row r="194" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J194" s="4"/>
+      <c r="L193" s="4"/>
+    </row>
+    <row r="194" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K194" s="4"/>
-    </row>
-    <row r="195" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J195" s="4"/>
+      <c r="L194" s="4"/>
+    </row>
+    <row r="195" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K195" s="4"/>
-    </row>
-    <row r="196" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J196" s="4"/>
+      <c r="L195" s="4"/>
+    </row>
+    <row r="196" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K196" s="4"/>
-    </row>
-    <row r="197" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J197" s="4"/>
+      <c r="L196" s="4"/>
+    </row>
+    <row r="197" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K197" s="4"/>
-    </row>
-    <row r="198" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J198" s="4"/>
+      <c r="L197" s="4"/>
+    </row>
+    <row r="198" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K198" s="4"/>
-    </row>
-    <row r="199" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J199" s="4"/>
+      <c r="L198" s="4"/>
+    </row>
+    <row r="199" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K199" s="4"/>
-    </row>
-    <row r="200" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J200" s="4"/>
+      <c r="L199" s="4"/>
+    </row>
+    <row r="200" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K200" s="4"/>
-    </row>
-    <row r="201" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J201" s="4"/>
+      <c r="L200" s="4"/>
+    </row>
+    <row r="201" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K201" s="4"/>
-    </row>
-    <row r="202" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J202" s="4"/>
+      <c r="L201" s="4"/>
+    </row>
+    <row r="202" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K202" s="4"/>
-    </row>
-    <row r="203" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J203" s="4"/>
+      <c r="L202" s="4"/>
+    </row>
+    <row r="203" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K203" s="4"/>
-    </row>
-    <row r="204" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J204" s="4"/>
+      <c r="L203" s="4"/>
+    </row>
+    <row r="204" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K204" s="4"/>
-    </row>
-    <row r="205" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J205" s="4"/>
+      <c r="L204" s="4"/>
+    </row>
+    <row r="205" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K205" s="4"/>
-    </row>
-    <row r="206" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J206" s="4"/>
+      <c r="L205" s="4"/>
+    </row>
+    <row r="206" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K206" s="4"/>
-    </row>
-    <row r="207" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J207" s="4"/>
+      <c r="L206" s="4"/>
+    </row>
+    <row r="207" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K207" s="4"/>
-    </row>
-    <row r="208" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J208" s="4"/>
+      <c r="L207" s="4"/>
+    </row>
+    <row r="208" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K208" s="4"/>
-    </row>
-    <row r="209" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J209" s="4"/>
+      <c r="L208" s="4"/>
+    </row>
+    <row r="209" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K209" s="4"/>
-    </row>
-    <row r="210" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J210" s="4"/>
+      <c r="L209" s="4"/>
+    </row>
+    <row r="210" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K210" s="4"/>
-    </row>
-    <row r="211" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J211" s="4"/>
+      <c r="L210" s="4"/>
+    </row>
+    <row r="211" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K211" s="4"/>
-    </row>
-    <row r="212" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J212" s="4"/>
+      <c r="L211" s="4"/>
+    </row>
+    <row r="212" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K212" s="4"/>
-    </row>
-    <row r="213" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J213" s="4"/>
+      <c r="L212" s="4"/>
+    </row>
+    <row r="213" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K213" s="4"/>
-    </row>
-    <row r="214" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J214" s="4"/>
+      <c r="L213" s="4"/>
+    </row>
+    <row r="214" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K214" s="4"/>
-    </row>
-    <row r="215" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J215" s="4"/>
+      <c r="L214" s="4"/>
+    </row>
+    <row r="215" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K215" s="4"/>
-    </row>
-    <row r="216" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J216" s="4"/>
+      <c r="L215" s="4"/>
+    </row>
+    <row r="216" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K216" s="4"/>
-    </row>
-    <row r="217" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J217" s="4"/>
+      <c r="L216" s="4"/>
+    </row>
+    <row r="217" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K217" s="4"/>
-    </row>
-    <row r="218" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J218" s="4"/>
+      <c r="L217" s="4"/>
+    </row>
+    <row r="218" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K218" s="4"/>
-    </row>
-    <row r="219" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J219" s="4"/>
+      <c r="L218" s="4"/>
+    </row>
+    <row r="219" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K219" s="4"/>
-    </row>
-    <row r="220" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J220" s="4"/>
+      <c r="L219" s="4"/>
+    </row>
+    <row r="220" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K220" s="4"/>
-    </row>
-    <row r="221" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J221" s="4"/>
+      <c r="L220" s="4"/>
+    </row>
+    <row r="221" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K221" s="4"/>
-    </row>
-    <row r="222" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J222" s="4"/>
+      <c r="L221" s="4"/>
+    </row>
+    <row r="222" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K222" s="4"/>
-    </row>
-    <row r="223" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J223" s="4"/>
+      <c r="L222" s="4"/>
+    </row>
+    <row r="223" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K223" s="4"/>
-    </row>
-    <row r="224" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J224" s="4"/>
+      <c r="L223" s="4"/>
+    </row>
+    <row r="224" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K224" s="4"/>
-    </row>
-    <row r="225" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J225" s="4"/>
+      <c r="L224" s="4"/>
+    </row>
+    <row r="225" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K225" s="4"/>
-    </row>
-    <row r="226" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J226" s="4"/>
+      <c r="L225" s="4"/>
+    </row>
+    <row r="226" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K226" s="4"/>
-    </row>
-    <row r="227" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J227" s="4"/>
+      <c r="L226" s="4"/>
+    </row>
+    <row r="227" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K227" s="4"/>
-    </row>
-    <row r="228" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J228" s="4"/>
+      <c r="L227" s="4"/>
+    </row>
+    <row r="228" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K228" s="4"/>
-    </row>
-    <row r="229" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J229" s="4"/>
+      <c r="L228" s="4"/>
+    </row>
+    <row r="229" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K229" s="4"/>
-    </row>
-    <row r="230" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J230" s="4"/>
+      <c r="L229" s="4"/>
+    </row>
+    <row r="230" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K230" s="4"/>
-    </row>
-    <row r="231" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J231" s="4"/>
+      <c r="L230" s="4"/>
+    </row>
+    <row r="231" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K231" s="4"/>
-    </row>
-    <row r="232" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J232" s="4"/>
+      <c r="L231" s="4"/>
+    </row>
+    <row r="232" spans="11:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K232" s="4"/>
-    </row>
-    <row r="233" spans="10:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="234" spans="10:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="235" spans="10:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="236" spans="10:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="237" spans="10:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="238" spans="10:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="239" spans="10:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="240" spans="10:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="L232" s="4"/>
+    </row>
+    <row r="233" spans="11:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="234" spans="11:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="235" spans="11:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="236" spans="11:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="237" spans="11:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="238" spans="11:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="239" spans="11:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="240" spans="11:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3810,39 +4381,64 @@
     <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:K26">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:L26">
     <sortCondition ref="C7:C26"/>
   </sortState>
+  <conditionalFormatting sqref="M7:M1048576">
+    <cfRule type="containsText" dxfId="11" priority="6" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",M7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",M7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N7:N1048576">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",N7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",N7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N7:N36">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="between">
+      <formula>0</formula>
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThanOrEqual">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F7" r:id="rId1" xr:uid="{5C949890-F12D-4585-BD0E-0D6CA3D34C18}"/>
-    <hyperlink ref="I9" r:id="rId2" xr:uid="{07871774-7A07-4E28-A3A0-332E05CC2948}"/>
-    <hyperlink ref="I8" r:id="rId3" xr:uid="{B9A0C95F-24A7-43A6-A8BB-E4A95E9E78EA}"/>
-    <hyperlink ref="I10" r:id="rId4" xr:uid="{008528E4-2E73-4B22-A454-B7776E85CA89}"/>
-    <hyperlink ref="I11" r:id="rId5" xr:uid="{324F76B0-D12E-4750-93A9-59D2686D370C}"/>
-    <hyperlink ref="I12" r:id="rId6" xr:uid="{749E0373-BC16-4DD6-AF6F-D0A47714E633}"/>
-    <hyperlink ref="I13" r:id="rId7" xr:uid="{05C33111-6193-4237-986A-0D815AD9D7EE}"/>
-    <hyperlink ref="I14" r:id="rId8" xr:uid="{952A618D-0450-485D-AC8E-872B06C6B31F}"/>
-    <hyperlink ref="I15" r:id="rId9" xr:uid="{D7B13C6F-7AE2-42BA-9AA3-54D011627C6E}"/>
-    <hyperlink ref="I16" r:id="rId10" xr:uid="{99503B9F-1AB6-4E44-9AE4-87FCDE5428CF}"/>
-    <hyperlink ref="I17" r:id="rId11" display="https://www.adafruit.com/product/2900" xr:uid="{53D6D7CA-5CA0-4A23-A6FF-E81E57F37A1C}"/>
-    <hyperlink ref="I18" r:id="rId12" xr:uid="{BE9CD5DF-B813-423C-BCA8-98D21964A730}"/>
-    <hyperlink ref="I19" r:id="rId13" display="https://www.parallax.com/product/4x4-matrix-membrane-keypad/" xr:uid="{C376B60A-63B8-4766-A189-F60A5A053F47}"/>
-    <hyperlink ref="I20" r:id="rId14" xr:uid="{DB8EC48B-A4EE-4AFF-841A-5B94A051C062}"/>
-    <hyperlink ref="I22" r:id="rId15" xr:uid="{3E9C6E8F-46CF-4D9A-9C37-42F571FE7445}"/>
-    <hyperlink ref="I21" r:id="rId16" xr:uid="{2A31938C-3DFB-4AD1-934C-6D9473ABDCDA}"/>
-    <hyperlink ref="I23" r:id="rId17" xr:uid="{58776D41-F733-4033-84E5-908234BE46F4}"/>
-    <hyperlink ref="I24" r:id="rId18" xr:uid="{EBE39A06-5EFF-4C3D-9DE9-ECA44899D8D5}"/>
-    <hyperlink ref="I25" r:id="rId19" xr:uid="{B360CDEC-4496-45AA-A02A-41B5F41B09F6}"/>
-    <hyperlink ref="I26" r:id="rId20" xr:uid="{2750C2C9-AAED-4807-921A-F2473CC7FC8C}"/>
-    <hyperlink ref="I27" r:id="rId21" xr:uid="{F15F62CD-0276-4CEA-9636-B110F6BE3512}"/>
-    <hyperlink ref="I28" r:id="rId22" xr:uid="{DCD57B2E-E3C2-466C-9FD3-5381281BF22F}"/>
-    <hyperlink ref="I29" r:id="rId23" xr:uid="{A4CEE88A-A5CA-488B-ADD2-695FA0C61EB8}"/>
-    <hyperlink ref="I30" r:id="rId24" xr:uid="{C2C48EA6-EB04-40C9-9258-4FDCEA06DF8F}"/>
-    <hyperlink ref="I31" r:id="rId25" display="https://www.adafruit.com/product/3405" xr:uid="{AB667FCB-D352-4AA8-BE36-51C0C69C1E4C}"/>
-    <hyperlink ref="I32" r:id="rId26" display="https://www.adafruit.com/product/385" xr:uid="{847F29FF-43D9-4C7C-B097-3ADCD7323010}"/>
-    <hyperlink ref="I34" r:id="rId27" display="https://www.adafruit.com/product/4918" xr:uid="{1B5501F5-A60E-4D2F-BE7D-FFF17B3F6067}"/>
-    <hyperlink ref="I35" r:id="rId28" xr:uid="{0B7A28CA-6C61-40A9-958E-D6F09791D987}"/>
-    <hyperlink ref="I36" r:id="rId29" xr:uid="{E8D2D2FF-9E7D-4097-AFD9-0BC587724D90}"/>
+    <hyperlink ref="G7" r:id="rId1" xr:uid="{5C949890-F12D-4585-BD0E-0D6CA3D34C18}"/>
+    <hyperlink ref="J9" r:id="rId2" xr:uid="{07871774-7A07-4E28-A3A0-332E05CC2948}"/>
+    <hyperlink ref="J8" r:id="rId3" xr:uid="{B9A0C95F-24A7-43A6-A8BB-E4A95E9E78EA}"/>
+    <hyperlink ref="J10" r:id="rId4" xr:uid="{008528E4-2E73-4B22-A454-B7776E85CA89}"/>
+    <hyperlink ref="J11" r:id="rId5" xr:uid="{324F76B0-D12E-4750-93A9-59D2686D370C}"/>
+    <hyperlink ref="J12" r:id="rId6" xr:uid="{749E0373-BC16-4DD6-AF6F-D0A47714E633}"/>
+    <hyperlink ref="J13" r:id="rId7" xr:uid="{05C33111-6193-4237-986A-0D815AD9D7EE}"/>
+    <hyperlink ref="J14" r:id="rId8" xr:uid="{952A618D-0450-485D-AC8E-872B06C6B31F}"/>
+    <hyperlink ref="J15" r:id="rId9" xr:uid="{D7B13C6F-7AE2-42BA-9AA3-54D011627C6E}"/>
+    <hyperlink ref="J16" r:id="rId10" xr:uid="{99503B9F-1AB6-4E44-9AE4-87FCDE5428CF}"/>
+    <hyperlink ref="J17" r:id="rId11" display="https://www.adafruit.com/product/2900" xr:uid="{53D6D7CA-5CA0-4A23-A6FF-E81E57F37A1C}"/>
+    <hyperlink ref="J18" r:id="rId12" xr:uid="{BE9CD5DF-B813-423C-BCA8-98D21964A730}"/>
+    <hyperlink ref="J19" r:id="rId13" display="https://www.parallax.com/product/4x4-matrix-membrane-keypad/" xr:uid="{C376B60A-63B8-4766-A189-F60A5A053F47}"/>
+    <hyperlink ref="J20" r:id="rId14" xr:uid="{DB8EC48B-A4EE-4AFF-841A-5B94A051C062}"/>
+    <hyperlink ref="J22" r:id="rId15" xr:uid="{3E9C6E8F-46CF-4D9A-9C37-42F571FE7445}"/>
+    <hyperlink ref="J21" r:id="rId16" xr:uid="{2A31938C-3DFB-4AD1-934C-6D9473ABDCDA}"/>
+    <hyperlink ref="J23" r:id="rId17" xr:uid="{58776D41-F733-4033-84E5-908234BE46F4}"/>
+    <hyperlink ref="J24" r:id="rId18" xr:uid="{EBE39A06-5EFF-4C3D-9DE9-ECA44899D8D5}"/>
+    <hyperlink ref="J25" r:id="rId19" xr:uid="{B360CDEC-4496-45AA-A02A-41B5F41B09F6}"/>
+    <hyperlink ref="J26" r:id="rId20" xr:uid="{2750C2C9-AAED-4807-921A-F2473CC7FC8C}"/>
+    <hyperlink ref="J27" r:id="rId21" xr:uid="{F15F62CD-0276-4CEA-9636-B110F6BE3512}"/>
+    <hyperlink ref="J28" r:id="rId22" xr:uid="{DCD57B2E-E3C2-466C-9FD3-5381281BF22F}"/>
+    <hyperlink ref="J29" r:id="rId23" xr:uid="{A4CEE88A-A5CA-488B-ADD2-695FA0C61EB8}"/>
+    <hyperlink ref="J30" r:id="rId24" xr:uid="{C2C48EA6-EB04-40C9-9258-4FDCEA06DF8F}"/>
+    <hyperlink ref="J31" r:id="rId25" display="https://www.adafruit.com/product/3405" xr:uid="{AB667FCB-D352-4AA8-BE36-51C0C69C1E4C}"/>
+    <hyperlink ref="J32" r:id="rId26" display="https://www.adafruit.com/product/385" xr:uid="{847F29FF-43D9-4C7C-B097-3ADCD7323010}"/>
+    <hyperlink ref="J34" r:id="rId27" display="https://www.adafruit.com/product/4918" xr:uid="{1B5501F5-A60E-4D2F-BE7D-FFF17B3F6067}"/>
+    <hyperlink ref="J35" r:id="rId28" xr:uid="{0B7A28CA-6C61-40A9-958E-D6F09791D987}"/>
+    <hyperlink ref="J36" r:id="rId29" xr:uid="{E8D2D2FF-9E7D-4097-AFD9-0BC587724D90}"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1.6666666666666701" bottom="1.6666666666666701" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId30"/>

</xml_diff>